<commit_message>
Add expenses column to the xlsx report
</commit_message>
<xml_diff>
--- a/Reports/XlsxReports/test.xlsx
+++ b/Reports/XlsxReports/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <x:si>
     <x:t>Vendor</x:t>
   </x:si>
@@ -22,22 +22,163 @@
     <x:t>Incomes</x:t>
   </x:si>
   <x:si>
+    <x:t>Expenses</x:t>
+  </x:si>
+  <x:si>
     <x:t>Taxes</x:t>
   </x:si>
   <x:si>
-    <x:t>Financial Result</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Item4</x:t>
+    <x:t>Financial Balance</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#31</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#34</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#43</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#46</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#47</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor#49</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -409,20 +550,21 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E6"/>
+  <x:dimension ref="A1:F52"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="8.250625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="11.280625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="9.120625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="6.760625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="15.450625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="9.850625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="10.860625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="16.830624999999998" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -435,61 +577,858 @@
       <x:c r="E2" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
+      <x:c r="F2" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="B3" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="C3" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="D3" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="E3" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
       <x:c r="B4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C4" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E4" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
+        <x:v>0.9088327</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="n">
+        <x:v>-0.9088327</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
       <x:c r="B5" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E5" s="0" t="n">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
+        <x:v>3.911868</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="n">
+        <x:v>-3.911868</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
       <x:c r="B6" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C6" s="0" t="n">
-        <x:v>1</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
-        <x:v>2</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E6" s="0" t="n">
-        <x:v>5</x:v>
+        <x:v>6.653493</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="n">
+        <x:v>-6.653493</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
+      <x:c r="B7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="n">
+        <x:v>11.83673</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="n">
+        <x:v>-11.83673</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6">
+      <x:c r="B8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="n">
+        <x:v>0.1675486</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="n">
+        <x:v>-0.1675486</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
+      <x:c r="B9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="n">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="n">
+        <x:v>2.771084</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="n">
+        <x:v>-2.771084</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
+      <x:c r="B10" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="n">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="n">
+        <x:v>1.041686</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="n">
+        <x:v>-1.041686</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="B11" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="n">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="n">
+        <x:v>11.90028</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="n">
+        <x:v>-11.90028</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
+      <x:c r="B12" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="n">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="n">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="n">
+        <x:v>0.6111052</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="n">
+        <x:v>-0.6111052</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6">
+      <x:c r="B13" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="n">
+        <x:v>2.22088</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="n">
+        <x:v>-2.22088</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="B14" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="n">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="n">
+        <x:v>110</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="n">
+        <x:v>23.86288</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="n">
+        <x:v>-23.86288</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
+      <x:c r="B15" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="n">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="n">
+        <x:v>120</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="n">
+        <x:v>0.6026739</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="n">
+        <x:v>-0.6026739</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="B16" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="n">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="n">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="n">
+        <x:v>7.460452</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="n">
+        <x:v>-7.460452</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="B17" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="n">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="n">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="n">
+        <x:v>10.23064</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="n">
+        <x:v>-10.23064</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="B18" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="n">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="n">
+        <x:v>150</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="n">
+        <x:v>36.40419</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="n">
+        <x:v>-36.40419</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="B19" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="n">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="n">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="n">
+        <x:v>37.48301</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="n">
+        <x:v>-37.48301</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="B20" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="n">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="n">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="n">
+        <x:v>20.34023</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="n">
+        <x:v>-20.34023</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="B21" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="n">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="n">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="n">
+        <x:v>18.43243</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="n">
+        <x:v>-18.43243</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="B22" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="n">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="n">
+        <x:v>190</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="n">
+        <x:v>54.79479</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="n">
+        <x:v>-54.79479</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="B23" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="n">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="n">
+        <x:v>200</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="n">
+        <x:v>0.5294945</x:v>
+      </x:c>
+      <x:c r="F23" s="0" t="n">
+        <x:v>-0.5294945</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="B24" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="n">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="n">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="n">
+        <x:v>58.52472</x:v>
+      </x:c>
+      <x:c r="F24" s="0" t="n">
+        <x:v>-58.52472</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="B25" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="n">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="n">
+        <x:v>220</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="n">
+        <x:v>59.10128</x:v>
+      </x:c>
+      <x:c r="F25" s="0" t="n">
+        <x:v>-59.10128</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="B26" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="n">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="n">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="n">
+        <x:v>43.58947</x:v>
+      </x:c>
+      <x:c r="F26" s="0" t="n">
+        <x:v>-43.58947</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="B27" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="n">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="n">
+        <x:v>240</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="n">
+        <x:v>23.26271</x:v>
+      </x:c>
+      <x:c r="F27" s="0" t="n">
+        <x:v>-23.26271</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="B28" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="n">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="n">
+        <x:v>250</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="n">
+        <x:v>36.48656</x:v>
+      </x:c>
+      <x:c r="F28" s="0" t="n">
+        <x:v>-36.48656</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="B29" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="n">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="n">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="n">
+        <x:v>34.152</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="n">
+        <x:v>-34.152</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="B30" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="n">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="n">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="n">
+        <x:v>65.44731</x:v>
+      </x:c>
+      <x:c r="F30" s="0" t="n">
+        <x:v>-65.44731</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="B31" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="n">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="n">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="n">
+        <x:v>17.36872</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="n">
+        <x:v>-17.36872</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="B32" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="n">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="n">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="n">
+        <x:v>39.68264</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="n">
+        <x:v>-39.68264</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="B33" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="n">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="n">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="n">
+        <x:v>60.30849</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="n">
+        <x:v>-60.30849</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="B34" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="n">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="n">
+        <x:v>310</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="n">
+        <x:v>8.42766</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="n">
+        <x:v>-8.42766</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="B35" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="n">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="n">
+        <x:v>320</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="n">
+        <x:v>72.64104</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="n">
+        <x:v>-72.64104</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="B36" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="n">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="n">
+        <x:v>330</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="n">
+        <x:v>78.01994</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="n">
+        <x:v>-78.01994</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="B37" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="n">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="n">
+        <x:v>340</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="n">
+        <x:v>13.99898</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="n">
+        <x:v>-13.99898</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="B38" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="n">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="n">
+        <x:v>350</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="n">
+        <x:v>69.16602</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="n">
+        <x:v>-69.16602</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="B39" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="n">
+        <x:v>38.56453</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="n">
+        <x:v>-38.56453</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="B40" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="n">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="n">
+        <x:v>370</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="n">
+        <x:v>107.7031</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="n">
+        <x:v>-107.7031</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="B41" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="n">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="n">
+        <x:v>380</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="n">
+        <x:v>59.80891</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="n">
+        <x:v>-59.80891</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="B42" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="n">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="n">
+        <x:v>390</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="n">
+        <x:v>29.29485</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="n">
+        <x:v>-29.29485</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="B43" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="n">
+        <x:v>400</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="n">
+        <x:v>400</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="n">
+        <x:v>18.16434</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="n">
+        <x:v>-18.16434</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="B44" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="n">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="n">
+        <x:v>410</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="n">
+        <x:v>114.2855</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="n">
+        <x:v>-114.2855</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="B45" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="n">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="n">
+        <x:v>420</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="n">
+        <x:v>118.7239</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="n">
+        <x:v>-118.7239</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6">
+      <x:c r="B46" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="n">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="n">
+        <x:v>430</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="n">
+        <x:v>64.25295</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="n">
+        <x:v>-64.25295</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6">
+      <x:c r="B47" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="n">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="n">
+        <x:v>440</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="n">
+        <x:v>62.8764</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="n">
+        <x:v>-62.8764</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6">
+      <x:c r="B48" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="n">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="n">
+        <x:v>450</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="n">
+        <x:v>68.83596</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="n">
+        <x:v>-68.83596</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6">
+      <x:c r="B49" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="n">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="n">
+        <x:v>460</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="n">
+        <x:v>128.883</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="n">
+        <x:v>-128.883</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6">
+      <x:c r="B50" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="n">
+        <x:v>470</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="n">
+        <x:v>470</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="n">
+        <x:v>113.976</x:v>
+      </x:c>
+      <x:c r="F50" s="0" t="n">
+        <x:v>-113.976</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6">
+      <x:c r="B51" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="n">
+        <x:v>480</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="n">
+        <x:v>480</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="n">
+        <x:v>50.29564</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="n">
+        <x:v>-50.29564</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:6">
+      <x:c r="B52" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="n">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="n">
+        <x:v>490</x:v>
+      </x:c>
+      <x:c r="E52" s="0" t="n">
+        <x:v>107.5889</x:v>
+      </x:c>
+      <x:c r="F52" s="0" t="n">
+        <x:v>-107.5889</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>